<commit_message>
Add Chart & Active Stream
</commit_message>
<xml_diff>
--- a/resources - streaming data/Stream_Table.xlsx
+++ b/resources - streaming data/Stream_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc640c57cda25b6/Desktop/Repo - Personal/Repo - TD API Client/td-ameritrade-python-api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8bc640c57cda25b6/Desktop/Repo - Personal/Repo - TD API Client/td-ameritrade-python-api/resources - streaming data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{964EAFF6-073A-4089-A129-8517468DB08E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{98CFF2B5-F5BB-4F78-8591-28E7215D42DF}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="8_{964EAFF6-073A-4089-A129-8517468DB08E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{29F7B932-1656-489A-8725-93A118A01B7F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1AFD0EED-8887-42F0-AEE4-FE4FD0BDECD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1AFD0EED-8887-42F0-AEE4-FE4FD0BDECD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="339">
   <si>
     <t>ields</t>
   </si>
@@ -1164,6 +1164,21 @@
   </si>
   <si>
     <t>3 = Message Data</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Chart Time</t>
+  </si>
+  <si>
+    <t>Chart Day</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +1989,8 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Roboto Light"/>
+        <name val="Roboto"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1992,6 +2008,78 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
         <name val="Roboto"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -2119,7 +2207,8 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Roboto Light"/>
+        <name val="Roboto"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2245,182 +2334,6 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
         <name val="Roboto"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -2429,11 +2342,77 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2448,34 +2427,70 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Roboto"/>
-        <family val="2"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Roboto Light"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2509,26 +2524,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{050F1F65-484A-49B3-9D6D-DFA80B5A068C}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="72" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{050F1F65-484A-49B3-9D6D-DFA80B5A068C}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:D7" xr:uid="{971E81A5-385A-4CA0-8D34-A20C670733A4}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{DEF12CB8-F39F-4748-B0FD-627CFD946398}" name="Table Name" dataDxfId="67"/>
-    <tableColumn id="1" xr3:uid="{394C2F56-A652-41FC-ADFC-633482479540}" name="Request" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{6E2307A4-5D8D-4D4D-AFC7-1E1489FEA36E}" name="Name" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{DC42DAF2-CE50-41A2-8EB2-279EFA8C8165}" name="Parameter" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{DEF12CB8-F39F-4748-B0FD-627CFD946398}" name="Table Name" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{394C2F56-A652-41FC-ADFC-633482479540}" name="Request" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{6E2307A4-5D8D-4D4D-AFC7-1E1489FEA36E}" name="Name" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{DC42DAF2-CE50-41A2-8EB2-279EFA8C8165}" name="Parameter" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3BC00CF-BB7D-44B9-91FD-AE6ECEE47FC9}" name="Table10" displayName="Table10" ref="A98:D109" totalsRowShown="0" headerRowDxfId="17" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3BC00CF-BB7D-44B9-91FD-AE6ECEE47FC9}" name="Table10" displayName="Table10" ref="A98:D109" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A98:D109" xr:uid="{629728F9-3590-4D81-B43D-4C025000A641}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1CBEC082-94A5-4142-A19F-3179B5E9ACE2}" name="Table Name" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{8B07619C-3896-4532-9AE8-27FC975ADC4B}" name="Request" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{1FC0DA7B-EB63-4F23-A6FF-92E9120EF735}" name="Value" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{DE8CBE8E-9D54-4AE5-AC7B-A64793C51BE5}" name="Description" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{1CBEC082-94A5-4142-A19F-3179B5E9ACE2}" name="Table Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{8B07619C-3896-4532-9AE8-27FC975ADC4B}" name="Request" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{1FC0DA7B-EB63-4F23-A6FF-92E9120EF735}" name="Value" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{DE8CBE8E-9D54-4AE5-AC7B-A64793C51BE5}" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2561,105 +2576,105 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B45F6481-94B2-43EF-ACD0-E63382B1B195}" name="Table2" displayName="Table2" ref="A9:D13" totalsRowShown="0" headerRowDxfId="71" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B45F6481-94B2-43EF-ACD0-E63382B1B195}" name="Table2" displayName="Table2" ref="A9:D13" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A9:D13" xr:uid="{4D7DC04F-44A8-4A32-AD5B-23E170159C23}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{9B4EF882-B43C-4306-B683-7FE8CC28272D}" name="Table Name" dataDxfId="62"/>
-    <tableColumn id="1" xr3:uid="{42571ECF-A33A-46E5-9E63-A54CBF2155E5}" name="Request" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{2F5A84EF-328C-4377-BA26-3F80E5339B49}" name="Name" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{E7B8DCA2-F0BE-42F1-ADAA-C0ACCA202E42}" name="Parameter" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{9B4EF882-B43C-4306-B683-7FE8CC28272D}" name="Table Name" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{42571ECF-A33A-46E5-9E63-A54CBF2155E5}" name="Request" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{2F5A84EF-328C-4377-BA26-3F80E5339B49}" name="Name" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{E7B8DCA2-F0BE-42F1-ADAA-C0ACCA202E42}" name="Parameter" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ADE64101-D026-43EE-8FE3-33FD7B89DA4B}" name="Table3" displayName="Table3" ref="A15:E46" totalsRowShown="0" headerRowDxfId="70" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ADE64101-D026-43EE-8FE3-33FD7B89DA4B}" name="Table3" displayName="Table3" ref="A15:E46" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A15:E46" xr:uid="{B5723AEA-C9DC-4B01-A016-609A79DD63FC}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{ADE88705-BC48-4A20-A5CC-26A652F0BCDC}" name="Table Name" dataDxfId="57"/>
-    <tableColumn id="1" xr3:uid="{61AD9E4F-5D7A-4AE7-B381-20193B17CAF7}" name="Service Name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{8680122A-52C2-4158-8DA4-D4235179CC96}" name="Description" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{6F4A7D51-5016-4EFF-9096-8252922DA8A8}" name="Delivery Type" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{35389CA0-4DF2-4AA5-86A2-5D85EC8AABAA}" name="Hours Available" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{ADE88705-BC48-4A20-A5CC-26A652F0BCDC}" name="Table Name" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{61AD9E4F-5D7A-4AE7-B381-20193B17CAF7}" name="Service Name" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{8680122A-52C2-4158-8DA4-D4235179CC96}" name="Description" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{6F4A7D51-5016-4EFF-9096-8252922DA8A8}" name="Delivery Type" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{35389CA0-4DF2-4AA5-86A2-5D85EC8AABAA}" name="Hours Available" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3986A3AF-EA1E-4328-96B7-52AAA6814E48}" name="Table4" displayName="Table4" ref="A48:E54" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3986A3AF-EA1E-4328-96B7-52AAA6814E48}" name="Table4" displayName="Table4" ref="A48:E54" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A48:E54" xr:uid="{355F9F3A-FF27-43A6-BDCB-84D02943FD76}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{228813D8-9BE4-4DF3-B4BE-0ECAD0B2A6C5}" name="Table Name" dataDxfId="40"/>
-    <tableColumn id="1" xr3:uid="{F70B8F8E-4EE5-437D-B861-D4A7757F1E45}" name="Service Name" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{53560722-56A0-4591-A382-8C3F6AF895DE}" name="Description" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{16DB8579-076A-4A54-8533-11B9094D630E}" name="Delivery Type" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{834E7FFC-4B30-44EF-8B36-3E58F2AD20C9}" name="Hours Available in ET" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{228813D8-9BE4-4DF3-B4BE-0ECAD0B2A6C5}" name="Table Name" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{F70B8F8E-4EE5-437D-B861-D4A7757F1E45}" name="Service Name" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{53560722-56A0-4591-A382-8C3F6AF895DE}" name="Description" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{16DB8579-076A-4A54-8533-11B9094D630E}" name="Delivery Type" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{834E7FFC-4B30-44EF-8B36-3E58F2AD20C9}" name="Hours Available in ET" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EB92C066-6A9D-4174-9447-E2512066DE7F}" name="Table5" displayName="Table5" ref="A56:C59" totalsRowShown="0" headerRowDxfId="69" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EB92C066-6A9D-4174-9447-E2512066DE7F}" name="Table5" displayName="Table5" ref="A56:C59" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A56:C59" xr:uid="{6BD3DB0D-0E2A-4B4F-99F5-8244C5C2CBC0}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{85CBD686-DB9E-4991-AAFA-3B26D9D134D4}" name="Table Name" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{6593C68A-4CF0-43F5-A8BE-350EDFE174FE}" name="Command" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{DFB7B07D-C1AC-4858-A8F3-10A7E23077F5}" name="Description" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{85CBD686-DB9E-4991-AAFA-3B26D9D134D4}" name="Table Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{6593C68A-4CF0-43F5-A8BE-350EDFE174FE}" name="Command" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{DFB7B07D-C1AC-4858-A8F3-10A7E23077F5}" name="Description" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9C43F62-8E8D-4DEB-8473-367720F6E382}" name="Table6" displayName="Table6" ref="A61:D83" totalsRowShown="0" headerRowDxfId="68" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9C43F62-8E8D-4DEB-8473-367720F6E382}" name="Table6" displayName="Table6" ref="A61:D83" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A61:D83" xr:uid="{E5141FF3-5451-41B4-9BD6-3C4446A7239B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D81493A1-48C5-4753-94A2-EE3F64C95D21}" name="Table Name" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{17020639-DE55-4AC3-B3E1-5145783B126C}" name="Request" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{65D6DDFB-DBBE-4FBA-B206-FBD19D7FE984}" name="Value" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{05DD5C56-53C9-4AB2-95E8-D379ABD9A57B}" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{D81493A1-48C5-4753-94A2-EE3F64C95D21}" name="Table Name" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{17020639-DE55-4AC3-B3E1-5145783B126C}" name="Request" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{65D6DDFB-DBBE-4FBA-B206-FBD19D7FE984}" name="Value" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{05DD5C56-53C9-4AB2-95E8-D379ABD9A57B}" name="Description" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{91C054AB-4215-4DE4-9305-4955B2CA45B1}" name="Table7" displayName="Table7" ref="A85:D87" totalsRowShown="0" headerRowDxfId="35" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{91C054AB-4215-4DE4-9305-4955B2CA45B1}" name="Table7" displayName="Table7" ref="A85:D87" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A85:D87" xr:uid="{963D1284-6095-44C3-935F-5A6ADF10AA3E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5571B7A9-B39A-4BE9-979F-035584AA992D}" name="Table Name" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{EEF7AF5F-362B-44F9-B678-EDE4A5BF73C7}" name="Name" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{1F287334-E74D-4209-BC23-C31CB3BAD3D2}" name="Type" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{8F1D617C-9D65-4A30-89FE-D2D229C48DC7}" name="Description" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{5571B7A9-B39A-4BE9-979F-035584AA992D}" name="Table Name" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{EEF7AF5F-362B-44F9-B678-EDE4A5BF73C7}" name="Name" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{1F287334-E74D-4209-BC23-C31CB3BAD3D2}" name="Type" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{8F1D617C-9D65-4A30-89FE-D2D229C48DC7}" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A32BB1E-26DA-47A8-A995-82CFE09EBCB5}" name="Table8" displayName="Table8" ref="A89:D92" totalsRowShown="0" headerRowDxfId="29" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A32BB1E-26DA-47A8-A995-82CFE09EBCB5}" name="Table8" displayName="Table8" ref="A89:D92" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A89:D92" xr:uid="{68120B83-DD4B-4DD5-93DB-8CA4331378A2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{57A17D15-5873-4DD2-8F70-6435E7032D0F}" name="Table Name" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{9101EFDA-8737-4073-8EDD-BD9B771A89E6}" name="Request" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{ABB03F3D-8657-4892-8CAA-467A3857912F}" name="Value" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{387A6806-DF19-4865-A31A-7EEAC523D953}" name="Description" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{57A17D15-5873-4DD2-8F70-6435E7032D0F}" name="Table Name" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9101EFDA-8737-4073-8EDD-BD9B771A89E6}" name="Request" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{ABB03F3D-8657-4892-8CAA-467A3857912F}" name="Value" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{387A6806-DF19-4865-A31A-7EEAC523D953}" name="Description" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{DACCE0D0-87C1-40B0-B92C-BF5C24818125}" name="Table9" displayName="Table9" ref="A94:D96" totalsRowShown="0" headerRowDxfId="23" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{DACCE0D0-87C1-40B0-B92C-BF5C24818125}" name="Table9" displayName="Table9" ref="A94:D96" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A94:D96" xr:uid="{5102153E-935F-4C13-A765-C3E747C029DF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{92AFF01A-EA1D-4A89-9D16-F22CB7603D5D}" name="Table Name" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{2157D949-A471-4698-BCA2-A6397062432F}" name="Name" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{891A3659-080C-4BDD-BD54-8093FF8E80E8}" name="Type" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{9585D152-1706-4A57-A240-81DB5320395F}" name="Description" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{92AFF01A-EA1D-4A89-9D16-F22CB7603D5D}" name="Table Name" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{2157D949-A471-4698-BCA2-A6397062432F}" name="Name" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{891A3659-080C-4BDD-BD54-8093FF8E80E8}" name="Type" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{9585D152-1706-4A57-A240-81DB5320395F}" name="Description" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2962,10 +2977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59C1DC4-B8F3-4057-AD31-8F11C4611F3E}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4246,6 +4261,78 @@
         <v>59</v>
       </c>
     </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>3</v>
+      </c>
+      <c r="C92" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>4</v>
+      </c>
+      <c r="C93" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>5</v>
+      </c>
+      <c r="C94" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>7</v>
+      </c>
+      <c r="C96" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>338</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4256,8 +4343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7E4B00-9847-4F62-AF79-4752A1C6F661}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>